<commit_message>
feat(css-classNotes): added HTML demos for selectors, box model, and position/z-index chore(notes): updated class_notes.xlsx with latest session details
</commit_message>
<xml_diff>
--- a/1_Materials/classNotes/class_notes.xlsx
+++ b/1_Materials/classNotes/class_notes.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\WebDevelopment\1_Materials\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2_TIME_College\SRET\WebDevelopment\1_Materials\classNotes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9780" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MongoDB" sheetId="1" r:id="rId1"/>
     <sheet name="HTML" sheetId="3" r:id="rId2"/>
+    <sheet name="CSS" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="312">
   <si>
     <t>DATABASE</t>
   </si>
@@ -785,12 +786,812 @@
   <si>
     <t>footer</t>
   </si>
+  <si>
+    <t>CSS</t>
+  </si>
+  <si>
+    <t>Selector Type</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Use Case</t>
+  </si>
+  <si>
+    <t>Element</t>
+  </si>
+  <si>
+    <t>p {}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Target all </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>&lt;p&gt;</t>
+    </r>
+  </si>
+  <si>
+    <t>Class</t>
+  </si>
+  <si>
+    <t>.card {}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Target elements with class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>card</t>
+    </r>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>#main {}</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Target one element with id </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>main</t>
+    </r>
+  </si>
+  <si>
+    <t>Grouping</t>
+  </si>
+  <si>
+    <t>h1, h2 {}</t>
+  </si>
+  <si>
+    <t>Apply same style to multiple tags</t>
+  </si>
+  <si>
+    <t>Descendant</t>
+  </si>
+  <si>
+    <t>.container p {}</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>.container &gt; p {}</t>
+  </si>
+  <si>
+    <t>Adjacent sibling</t>
+  </si>
+  <si>
+    <t>h1 + p {}</t>
+  </si>
+  <si>
+    <t>Pseudo-class</t>
+  </si>
+  <si>
+    <t>a:hover {}</t>
+  </si>
+  <si>
+    <t>Adds hover effect on anchor</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>input[type="text"] {}</t>
+  </si>
+  <si>
+    <t>Targets text inputs only</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Selectors &amp; Measurement Units
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Foundation for targeting and sizing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2. Box Model</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– Critical for layout control and spacing</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>3. Position &amp; Z-index</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– Real-world layout control, stacking</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>4. Flexbox</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– 1D layout hero, dynamic UI building</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>5. Grid</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– 2D layout powerhouse, modern layouts</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>6. Transitions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– Micro-interactions, polish</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>7. Animations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– Engaging visuals</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>8. Media Queries</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+– Responsive design magic</t>
+    </r>
+  </si>
+  <si>
+    <t>MEASUREMENT UNITS</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>px</t>
+  </si>
+  <si>
+    <t>Fixed size</t>
+  </si>
+  <si>
+    <t>width: 300px</t>
+  </si>
+  <si>
+    <t>%</t>
+  </si>
+  <si>
+    <t>Relative to parent</t>
+  </si>
+  <si>
+    <t>width: 50%</t>
+  </si>
+  <si>
+    <t>em</t>
+  </si>
+  <si>
+    <t>Relative to parent font size</t>
+  </si>
+  <si>
+    <t>padding: 2em</t>
+  </si>
+  <si>
+    <t>rem</t>
+  </si>
+  <si>
+    <t>Relative to root font size</t>
+  </si>
+  <si>
+    <t>font-size: 1.5rem</t>
+  </si>
+  <si>
+    <t>vh/vw</t>
+  </si>
+  <si>
+    <t>Viewport height/width</t>
+  </si>
+  <si>
+    <t>height: 100vh</t>
+  </si>
+  <si>
+    <t>BOX MODEL</t>
+  </si>
+  <si>
+    <r>
+      <t>Content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Actual text/image inside the box</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Padding</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Space </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>inside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the box, around content</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Border</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Edge around the padding</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Margin</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> – Space </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>outside</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> the box, separating it from others</t>
+    </r>
+  </si>
+  <si>
+    <t>box-sizing</t>
+  </si>
+  <si>
+    <t>Feature</t>
+  </si>
+  <si>
+    <t>Actual rendered size</t>
+  </si>
+  <si>
+    <t>width + padding + border</t>
+  </si>
+  <si>
+    <t>Layout predictability</t>
+  </si>
+  <si>
+    <t>Less intuitive (can overflow if padding/border added)</t>
+  </si>
+  <si>
+    <t>Very intuitive for spacing/layout</t>
+  </si>
+  <si>
+    <t>Default behavior in CSS</t>
+  </si>
+  <si>
+    <t>Common use case</t>
+  </si>
+  <si>
+    <t>Learning internals / default browser behavior</t>
+  </si>
+  <si>
+    <t>Production UI, grid/flex layouts</t>
+  </si>
+  <si>
+    <r>
+      <t>content-box</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (default)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>border-box</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (modern layout favorite)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">What </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sets</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Only the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>content</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> area</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Total size = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>content + padding + border</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fits in </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>width</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Exactly the </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> you set</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Default box-sizing (</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>box-sizing: content-box</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You must set </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>box-sizing: border-box</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> manually (or globally)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Targets </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> inside </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>.container</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Targets </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>direct</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> children</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Targets </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>p</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> immediately after </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>h1</t>
+    </r>
+  </si>
+  <si>
+    <t>POSITION</t>
+  </si>
+  <si>
+    <t>Position Type</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>Default — normal flow</t>
+  </si>
+  <si>
+    <t>relative</t>
+  </si>
+  <si>
+    <t>Offsets from its original position</t>
+  </si>
+  <si>
+    <t>absolute</t>
+  </si>
+  <si>
+    <t>fixed</t>
+  </si>
+  <si>
+    <t>sticky</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Positioned relative to the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>nearest positioned ancestor</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Relative to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>viewport</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> — doesn’t scroll</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Acts like </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>relative</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, but sticks on scroll (based on threshold)</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -823,6 +1624,40 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -861,7 +1696,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -872,13 +1707,299 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="26">
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -1015,14 +2136,61 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="A14:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="rollNo" dataDxfId="4"/>
-    <tableColumn id="2" name="name" dataDxfId="3"/>
-    <tableColumn id="3" name="mobile" dataDxfId="2"/>
-    <tableColumn id="4" name="email" dataDxfId="1" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="deptNo" dataDxfId="0"/>
+    <tableColumn id="1" name="rollNo" dataDxfId="23"/>
+    <tableColumn id="2" name="name" dataDxfId="22"/>
+    <tableColumn id="3" name="mobile" dataDxfId="21"/>
+    <tableColumn id="4" name="email" dataDxfId="20" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="deptNo" dataDxfId="19"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C26:E35" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+  <autoFilter ref="C26:E35"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Selector Type" dataDxfId="8"/>
+    <tableColumn id="2" name="Example" dataDxfId="7"/>
+    <tableColumn id="3" name="Use Case" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C40:E45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+  <autoFilter ref="C40:E45"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Unit" dataDxfId="13"/>
+    <tableColumn id="2" name="Use Case" dataDxfId="12"/>
+    <tableColumn id="3" name="Example" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C59:E64" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="C59:E64"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Feature" dataDxfId="18"/>
+    <tableColumn id="2" name="content-box (default)" dataDxfId="17"/>
+    <tableColumn id="3" name="border-box (modern layout favorite)" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C69:D74" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+  <autoFilter ref="C69:D74"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Position Type" dataDxfId="3"/>
+    <tableColumn id="2" name="Description" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1293,11 +2461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+    <sheetView topLeftCell="A56" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
       <selection activeCell="B70" sqref="B70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" style="1" customWidth="1"/>
@@ -1308,12 +2476,12 @@
     <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11">
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1330,7 +2498,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11">
       <c r="F5" s="2" t="s">
         <v>5</v>
       </c>
@@ -1338,7 +2506,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11">
       <c r="F6" s="2" t="s">
         <v>6</v>
       </c>
@@ -1346,7 +2514,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11">
       <c r="F7" s="1" t="s">
         <v>7</v>
       </c>
@@ -1360,7 +2528,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11">
       <c r="B9" s="2" t="s">
         <v>13</v>
       </c>
@@ -1368,7 +2536,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11">
       <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1376,7 +2544,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11">
       <c r="B12" s="1" t="s">
         <v>32</v>
       </c>
@@ -1384,7 +2552,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="5" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" s="5" customFormat="1" ht="28.8">
       <c r="A13" s="5" t="s">
         <v>20</v>
       </c>
@@ -1401,7 +2569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -1421,7 +2589,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11">
       <c r="A15" s="4">
         <v>1</v>
       </c>
@@ -1441,7 +2609,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11">
       <c r="A16" s="4">
         <v>2</v>
       </c>
@@ -1461,7 +2629,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:3">
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
@@ -1469,27 +2637,27 @@
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:3" ht="86.4">
       <c r="B20" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="22" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3" ht="57.6">
       <c r="B22" s="5" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:3" ht="86.4">
       <c r="B24" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:3" ht="115.2">
       <c r="B25" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:6">
       <c r="B34" s="2" t="s">
         <v>14</v>
       </c>
@@ -1503,7 +2671,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:6">
       <c r="C35" s="1" t="s">
         <v>36</v>
       </c>
@@ -1514,7 +2682,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:6">
       <c r="C36" s="3" t="s">
         <v>40</v>
       </c>
@@ -1525,12 +2693,12 @@
         <v>44</v>
       </c>
     </row>
-    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:6">
       <c r="B41" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:6">
       <c r="B43" s="1" t="s">
         <v>46</v>
       </c>
@@ -1538,7 +2706,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:6">
       <c r="B44" s="1" t="s">
         <v>47</v>
       </c>
@@ -1546,7 +2714,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:6">
       <c r="B45" s="1" t="s">
         <v>48</v>
       </c>
@@ -1554,7 +2722,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:6">
       <c r="B46" s="1" t="s">
         <v>49</v>
       </c>
@@ -1562,12 +2730,12 @@
         <v>52</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:4">
       <c r="B51" s="1" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:4">
       <c r="B52" s="1" t="s">
         <v>54</v>
       </c>
@@ -1575,7 +2743,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:4">
       <c r="B53" s="1" t="s">
         <v>56</v>
       </c>
@@ -1583,12 +2751,12 @@
         <v>57</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:4">
       <c r="B56" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="57" spans="2:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:4" s="2" customFormat="1">
       <c r="B57" s="2" t="s">
         <v>119</v>
       </c>
@@ -1596,7 +2764,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:4">
       <c r="B58" s="1" t="s">
         <v>59</v>
       </c>
@@ -1604,7 +2772,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="59" spans="2:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:4" ht="43.2">
       <c r="B59" s="1" t="s">
         <v>63</v>
       </c>
@@ -1615,7 +2783,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:4">
       <c r="B60" s="1" t="s">
         <v>61</v>
       </c>
@@ -1623,12 +2791,12 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:4">
       <c r="B63" s="1" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:4">
       <c r="B64" s="1" t="s">
         <v>121</v>
       </c>
@@ -1636,17 +2804,17 @@
         <v>120</v>
       </c>
     </row>
-    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:6">
       <c r="B65" s="1" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:6">
       <c r="B69" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:6">
       <c r="B71" s="1" t="s">
         <v>68</v>
       </c>
@@ -1654,7 +2822,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:6">
       <c r="B72" s="1" t="s">
         <v>69</v>
       </c>
@@ -1662,7 +2830,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:6">
       <c r="B73" s="1" t="s">
         <v>72</v>
       </c>
@@ -1670,12 +2838,12 @@
         <v>84</v>
       </c>
     </row>
-    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:6">
       <c r="B75" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:6">
       <c r="B77" s="1" t="s">
         <v>92</v>
       </c>
@@ -1686,7 +2854,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:6">
       <c r="B78" s="1" t="s">
         <v>77</v>
       </c>
@@ -1694,7 +2862,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:6">
       <c r="B79" s="1" t="s">
         <v>73</v>
       </c>
@@ -1705,7 +2873,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:6">
       <c r="C80" s="1" t="s">
         <v>75</v>
       </c>
@@ -1716,17 +2884,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:4">
       <c r="D81" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:4">
       <c r="D82" s="1" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="83" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:4">
       <c r="B83" s="1" t="s">
         <v>76</v>
       </c>
@@ -1734,12 +2902,12 @@
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:4">
       <c r="B84" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="86" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:4">
       <c r="B86" s="1" t="s">
         <v>79</v>
       </c>
@@ -1750,7 +2918,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="87" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:4">
       <c r="B87" s="1" t="s">
         <v>60</v>
       </c>
@@ -1761,7 +2929,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="88" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:4">
       <c r="B88" s="1" t="s">
         <v>59</v>
       </c>
@@ -1772,12 +2940,12 @@
         <v>102</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:4">
       <c r="B90" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:4">
       <c r="B92" s="1" t="s">
         <v>93</v>
       </c>
@@ -1788,7 +2956,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:4">
       <c r="B93" s="1" t="s">
         <v>94</v>
       </c>
@@ -1796,17 +2964,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:4">
       <c r="B94" s="1" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="96" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:4">
       <c r="C96" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5">
       <c r="B98" s="1" t="s">
         <v>103</v>
       </c>
@@ -1814,12 +2982,12 @@
         <v>104</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:5">
       <c r="B102" s="2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:5">
       <c r="B104" s="1" t="s">
         <v>106</v>
       </c>
@@ -1827,7 +2995,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:5">
       <c r="B105" s="1" t="s">
         <v>107</v>
       </c>
@@ -1835,7 +3003,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:5">
       <c r="B106" s="1" t="s">
         <v>105</v>
       </c>
@@ -1843,13 +3011,13 @@
         <v>126</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:5">
       <c r="B107" s="2"/>
       <c r="E107" s="1" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:5">
       <c r="B108" s="1" t="s">
         <v>108</v>
       </c>
@@ -1858,17 +3026,17 @@
       </c>
       <c r="D108" s="2"/>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:5">
       <c r="C109" s="1" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:5">
       <c r="B112" s="2" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:3">
       <c r="B114" s="1" t="s">
         <v>113</v>
       </c>
@@ -1876,7 +3044,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:3">
       <c r="B115" s="5" t="s">
         <v>114</v>
       </c>
@@ -1884,12 +3052,12 @@
         <v>115</v>
       </c>
     </row>
-    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:3">
       <c r="B118" s="2" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="120" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:3" ht="28.8">
       <c r="A120" s="1" t="s">
         <v>134</v>
       </c>
@@ -1900,7 +3068,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:3">
       <c r="A121" s="1" t="s">
         <v>135</v>
       </c>
@@ -1911,7 +3079,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:3">
       <c r="A122" s="1" t="s">
         <v>136</v>
       </c>
@@ -1922,22 +3090,22 @@
         <v>133</v>
       </c>
     </row>
-    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:3">
       <c r="B124" s="3" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:3">
       <c r="B125" s="3" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="129" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:4">
       <c r="B129" s="2" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="132" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:4">
       <c r="B132" s="1" t="s">
         <v>144</v>
       </c>
@@ -1945,17 +3113,17 @@
         <v>145</v>
       </c>
     </row>
-    <row r="134" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:4">
       <c r="B134" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="135" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:4">
       <c r="B135" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="138" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:4">
       <c r="B138" s="1" t="s">
         <v>149</v>
       </c>
@@ -1966,7 +3134,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="139" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:4">
       <c r="B139" s="1" t="s">
         <v>152</v>
       </c>
@@ -1977,22 +3145,22 @@
         <v>143</v>
       </c>
     </row>
-    <row r="142" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:4">
       <c r="B142" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="143" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:4">
       <c r="B143" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="144" spans="2:4" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:4">
       <c r="B144" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:3">
       <c r="B147" s="1" t="s">
         <v>118</v>
       </c>
@@ -2000,12 +3168,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:3">
       <c r="B149" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:3">
       <c r="B150" s="1" t="s">
         <v>154</v>
       </c>
@@ -2013,7 +3181,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="151" spans="2:3">
       <c r="B151" s="1" t="s">
         <v>155</v>
       </c>
@@ -2021,12 +3189,12 @@
         <v>159</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="152" spans="2:3">
       <c r="B152" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="153" spans="2:3">
       <c r="B153" s="1" t="s">
         <v>157</v>
       </c>
@@ -2055,19 +3223,19 @@
       <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="1"/>
     <col min="2" max="2" width="11.6640625" style="1" customWidth="1"/>
     <col min="3" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:10">
       <c r="B2" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:10">
       <c r="F3" s="1" t="s">
         <v>162</v>
       </c>
@@ -2078,7 +3246,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:10">
       <c r="B4" s="1" t="s">
         <v>165</v>
       </c>
@@ -2092,17 +3260,17 @@
         <v>168</v>
       </c>
     </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:10">
       <c r="B5" s="1" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:10">
       <c r="B6" s="1" t="s">
         <v>170</v>
       </c>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10">
       <c r="B7" s="1" t="s">
         <v>171</v>
       </c>
@@ -2113,17 +3281,17 @@
         <v>173</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10">
       <c r="B8" s="1" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10">
       <c r="B11" s="2" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10">
       <c r="B13" s="1" t="s">
         <v>176</v>
       </c>
@@ -2131,7 +3299,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10">
       <c r="B15" s="1" t="s">
         <v>178</v>
       </c>
@@ -2139,7 +3307,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10">
       <c r="B16" s="1" t="s">
         <v>180</v>
       </c>
@@ -2147,12 +3315,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:3">
       <c r="B19" s="2" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="21" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:3">
       <c r="B21" s="1" t="s">
         <v>183</v>
       </c>
@@ -2160,7 +3328,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:3">
       <c r="B22" s="1" t="s">
         <v>185</v>
       </c>
@@ -2168,7 +3336,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:3">
       <c r="B23" s="1" t="s">
         <v>187</v>
       </c>
@@ -2176,12 +3344,12 @@
         <v>188</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:3">
       <c r="B26" s="2" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:3">
       <c r="B28" s="1" t="s">
         <v>190</v>
       </c>
@@ -2189,7 +3357,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="29" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:3">
       <c r="B29" s="1" t="s">
         <v>192</v>
       </c>
@@ -2197,7 +3365,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="30" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:3">
       <c r="B30" s="1" t="s">
         <v>194</v>
       </c>
@@ -2205,7 +3373,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="31" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:3">
       <c r="B31" s="1" t="s">
         <v>70</v>
       </c>
@@ -2213,7 +3381,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="32" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:3">
       <c r="B32" s="1" t="s">
         <v>184</v>
       </c>
@@ -2221,7 +3389,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:3">
       <c r="B33" s="1" t="s">
         <v>186</v>
       </c>
@@ -2229,7 +3397,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:3">
       <c r="B34" s="1" t="s">
         <v>188</v>
       </c>
@@ -2237,12 +3405,12 @@
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:3">
       <c r="B36" s="2" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:3">
       <c r="B38" s="1" t="s">
         <v>201</v>
       </c>
@@ -2250,7 +3418,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:3">
       <c r="B39" s="1" t="s">
         <v>203</v>
       </c>
@@ -2258,7 +3426,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:3">
       <c r="B40" s="1" t="s">
         <v>205</v>
       </c>
@@ -2266,7 +3434,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:3">
       <c r="B41" s="1" t="s">
         <v>207</v>
       </c>
@@ -2274,7 +3442,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:3">
       <c r="B42" s="1" t="s">
         <v>209</v>
       </c>
@@ -2282,42 +3450,42 @@
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:3">
       <c r="B45" s="2" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:3">
       <c r="B47" s="1" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:3">
       <c r="B48" s="1" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:2">
       <c r="B49" s="1" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:2">
       <c r="B50" s="1" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:2">
       <c r="B51" s="1" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:2">
       <c r="B52" s="1" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:2">
       <c r="B53" s="1" t="s">
         <v>218</v>
       </c>
@@ -2326,4 +3494,444 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E74"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="28.21875" style="5" customWidth="1"/>
+    <col min="3" max="3" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="39.109375" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="2" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="57.6">
+      <c r="B3" s="9" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="B4" s="10"/>
+    </row>
+    <row r="5" spans="1:2" ht="43.2">
+      <c r="B5" s="9" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" s="10"/>
+    </row>
+    <row r="7" spans="1:2" ht="43.2">
+      <c r="B7" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="B8" s="10"/>
+    </row>
+    <row r="9" spans="1:2" ht="43.2">
+      <c r="B9" s="9" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" s="10"/>
+    </row>
+    <row r="11" spans="1:2" ht="43.2">
+      <c r="B11" s="9" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="B12" s="10"/>
+    </row>
+    <row r="13" spans="1:2" ht="28.8">
+      <c r="B13" s="9" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:2" ht="28.8">
+      <c r="B15" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" s="10"/>
+    </row>
+    <row r="17" spans="1:5" ht="28.8">
+      <c r="B17" s="9" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="2">
+        <v>1</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="15" customHeight="1">
+      <c r="C26" s="13" t="s">
+        <v>220</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>221</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" ht="15" customHeight="1">
+      <c r="C27" s="15" t="s">
+        <v>223</v>
+      </c>
+      <c r="D27" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="E27" s="15" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="15" customHeight="1">
+      <c r="C28" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D28" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="E28" s="15" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="15" customHeight="1">
+      <c r="C29" s="15" t="s">
+        <v>229</v>
+      </c>
+      <c r="D29" s="8" t="s">
+        <v>230</v>
+      </c>
+      <c r="E29" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="15" customHeight="1">
+      <c r="C30" s="15" t="s">
+        <v>232</v>
+      </c>
+      <c r="D30" s="8" t="s">
+        <v>233</v>
+      </c>
+      <c r="E30" s="15" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" ht="15" customHeight="1">
+      <c r="C31" s="15" t="s">
+        <v>235</v>
+      </c>
+      <c r="D31" s="8" t="s">
+        <v>236</v>
+      </c>
+      <c r="E31" s="15" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" ht="15" customHeight="1">
+      <c r="C32" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D32" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="E32" s="15" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" ht="15" customHeight="1">
+      <c r="C33" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D33" s="8" t="s">
+        <v>240</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" ht="15" customHeight="1">
+      <c r="C34" s="15" t="s">
+        <v>241</v>
+      </c>
+      <c r="D34" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="E34" s="15" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" ht="15" customHeight="1">
+      <c r="C35" s="15" t="s">
+        <v>244</v>
+      </c>
+      <c r="D35" s="8" t="s">
+        <v>245</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5">
+      <c r="B38" s="11" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5">
+      <c r="C40" s="13" t="s">
+        <v>256</v>
+      </c>
+      <c r="D40" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="E40" s="13" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5">
+      <c r="C41" s="8" t="s">
+        <v>257</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>258</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="42" spans="2:5">
+      <c r="C42" s="8" t="s">
+        <v>260</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>261</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="43" spans="2:5" ht="27.6">
+      <c r="C43" s="8" t="s">
+        <v>263</v>
+      </c>
+      <c r="D43" s="15" t="s">
+        <v>264</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="44" spans="2:5" ht="27.6">
+      <c r="C44" s="8" t="s">
+        <v>266</v>
+      </c>
+      <c r="D44" s="15" t="s">
+        <v>267</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="45" spans="2:5" ht="27.6">
+      <c r="C45" s="8" t="s">
+        <v>269</v>
+      </c>
+      <c r="D45" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" s="2">
+        <v>2</v>
+      </c>
+      <c r="B49" s="11" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28.8">
+      <c r="B51" s="11" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="28.8">
+      <c r="B53" s="11" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" ht="28.8">
+      <c r="B55" s="11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" ht="28.8">
+      <c r="B57" s="11" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="C58" s="2" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" ht="27.6">
+      <c r="C59" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="D59" s="12" t="s">
+        <v>288</v>
+      </c>
+      <c r="E59" s="12" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" ht="27.6">
+      <c r="C60" s="14" t="s">
+        <v>290</v>
+      </c>
+      <c r="D60" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="E60" s="15" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" ht="27.6">
+      <c r="C61" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>280</v>
+      </c>
+      <c r="E61" s="15" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" ht="55.2">
+      <c r="C62" s="14" t="s">
+        <v>281</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>282</v>
+      </c>
+      <c r="E62" s="15" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" ht="41.4">
+      <c r="C63" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D63" s="15" t="s">
+        <v>294</v>
+      </c>
+      <c r="E63" s="15" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" ht="41.4">
+      <c r="C64" s="14" t="s">
+        <v>285</v>
+      </c>
+      <c r="D64" s="15" t="s">
+        <v>286</v>
+      </c>
+      <c r="E64" s="15" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="2">
+        <v>3</v>
+      </c>
+      <c r="B68" s="11" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="C69" s="13" t="s">
+        <v>300</v>
+      </c>
+      <c r="D69" s="13" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="27.6">
+      <c r="C70" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D70" s="15" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="27.6">
+      <c r="C71" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="D71" s="15" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="41.4">
+      <c r="C72" s="8" t="s">
+        <v>306</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="41.4">
+      <c r="C73" s="8" t="s">
+        <v>307</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="55.2">
+      <c r="C74" s="8" t="s">
+        <v>308</v>
+      </c>
+      <c r="D74" s="15" t="s">
+        <v>311</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <tableParts count="4">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId5"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
feat(css-classNotes): added flexbox and grid layout demo files feat(html-classNotes): created index.html for HTML demos chore(notes): updated class_notes.xlsx with latest topics
</commit_message>
<xml_diff>
--- a/1_Materials/classNotes/class_notes.xlsx
+++ b/1_Materials/classNotes/class_notes.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="378">
   <si>
     <t>DATABASE</t>
   </si>
@@ -727,9 +727,6 @@
     <t>id selector</t>
   </si>
   <si>
-    <t>type</t>
-  </si>
-  <si>
     <t>ADVANCED TAGS</t>
   </si>
   <si>
@@ -1585,13 +1582,576 @@
       </rPr>
       <t>, but sticks on scroll (based on threshold)</t>
     </r>
+  </si>
+  <si>
+    <t>client url</t>
+  </si>
+  <si>
+    <t>react js</t>
+  </si>
+  <si>
+    <t>attributes</t>
+  </si>
+  <si>
+    <t>blood donation</t>
+  </si>
+  <si>
+    <t>www.live-saver.com</t>
+  </si>
+  <si>
+    <t>SCSS: bootstrap, tailwind</t>
+  </si>
+  <si>
+    <t>FLEX</t>
+  </si>
+  <si>
+    <t>Core Concepts</t>
+  </si>
+  <si>
+    <r>
+      <t>Default main axis:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> horizontal (left → right)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You can flip direction with </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>flex-direction</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parent → </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>display: flex</t>
+    </r>
+  </si>
+  <si>
+    <t>Main Axis &amp; Cross Axis</t>
+  </si>
+  <si>
+    <t>Property</t>
+  </si>
+  <si>
+    <t>display: flex</t>
+  </si>
+  <si>
+    <t>Enables flexbox layout</t>
+  </si>
+  <si>
+    <t>flex-direction</t>
+  </si>
+  <si>
+    <r>
+      <t>row</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (default), </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>row-reverse</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, etc.</t>
+    </r>
+  </si>
+  <si>
+    <t>justify-content</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aligns items </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>horizontally</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (main axis)</t>
+    </r>
+  </si>
+  <si>
+    <t>align-items</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Aligns items </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>vertically</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (cross axis)</t>
+    </r>
+  </si>
+  <si>
+    <t>flex-wrap</t>
+  </si>
+  <si>
+    <t>Allows items to wrap to new lines</t>
+  </si>
+  <si>
+    <t>flex-grow</t>
+  </si>
+  <si>
+    <t>Controls how much space to take</t>
+  </si>
+  <si>
+    <t>flex-shrink</t>
+  </si>
+  <si>
+    <t>Controls how much to shrink</t>
+  </si>
+  <si>
+    <t>flex-basis</t>
+  </si>
+  <si>
+    <t>Initial size</t>
+  </si>
+  <si>
+    <r>
+      <t>flex</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (shorthand)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Combines above: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>flex: 1</t>
+    </r>
+  </si>
+  <si>
+    <t>PARENT(Flex Container)</t>
+  </si>
+  <si>
+    <t>CHILD(Flex Item)</t>
+  </si>
+  <si>
+    <t>GRID</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Parent = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Grid Container</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Children = </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Grid Items</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>2D layout system</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: controls </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rows + columns</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">You define layout using </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>tracks</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (rows/columns), </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>areas</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>gaps</t>
+    </r>
+  </si>
+  <si>
+    <t>Purpose</t>
+  </si>
+  <si>
+    <t>grid-template-columns</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Defines columns (e.g. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>1fr 1fr 1fr</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>grid-template-rows</t>
+  </si>
+  <si>
+    <t>Defines rows (optional)</t>
+  </si>
+  <si>
+    <t>gap</t>
+  </si>
+  <si>
+    <t>Adds spacing between rows/columns</t>
+  </si>
+  <si>
+    <t>grid-template-areas</t>
+  </si>
+  <si>
+    <t>Optional named layout zones</t>
+  </si>
+  <si>
+    <r>
+      <t>place-items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> or </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>align-items</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> + </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>justify-items</t>
+    </r>
+  </si>
+  <si>
+    <t>Align grid items</t>
+  </si>
+  <si>
+    <t>Parent(grid container)</t>
+  </si>
+  <si>
+    <t>Child(grid item)</t>
+  </si>
+  <si>
+    <r>
+      <t>grid-column</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> / </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>grid-row</t>
+    </r>
+  </si>
+  <si>
+    <t>Manual positioning (start / end line)</t>
+  </si>
+  <si>
+    <t>grid-area</t>
+  </si>
+  <si>
+    <t>Assign named area</t>
+  </si>
+  <si>
+    <r>
+      <t>place-self</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>align-self</t>
+    </r>
+  </si>
+  <si>
+    <t>Individual alignment</t>
+  </si>
+  <si>
+    <t>usage</t>
+  </si>
+  <si>
+    <t>Grid Magic</t>
+  </si>
+  <si>
+    <t>Dashboard Layout</t>
+  </si>
+  <si>
+    <t>Multiple rows/columns</t>
+  </si>
+  <si>
+    <t>Photo Gallery</t>
+  </si>
+  <si>
+    <t>Responsive with auto-fit</t>
+  </si>
+  <si>
+    <t>Split Page</t>
+  </si>
+  <si>
+    <t>Sidebar + main content</t>
+  </si>
+  <si>
+    <t>CSS-Only Layouts</t>
+  </si>
+  <si>
+    <t>Skip flex nesting madness</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="10">
+  <fonts count="14">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1662,8 +2222,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1681,6 +2266,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1691,12 +2281,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1731,23 +2322,60 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="42">
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1760,12 +2388,150 @@
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
-        <sz val="10"/>
+        <sz val="11"/>
         <color theme="1"/>
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1836,25 +2602,6 @@
         <sz val="10"/>
         <color theme="1"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial Unicode MS"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1866,7 +2613,6 @@
         <sz val="10"/>
         <color theme="1"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1881,21 +2627,25 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
-        <i val="0"/>
         <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
       </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+      </font>
     </dxf>
     <dxf>
       <font>
@@ -1958,14 +2708,21 @@
     </dxf>
     <dxf>
       <font>
+        <b/>
+        <i val="0"/>
         <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
         <vertAlign val="baseline"/>
         <sz val="10"/>
         <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1977,6 +2734,25 @@
         <sz val="10"/>
         <color theme="1"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1988,6 +2764,7 @@
         <sz val="10"/>
         <color theme="1"/>
       </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -1999,6 +2776,24 @@
         <sz val="10"/>
         <color theme="1"/>
       </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2136,61 +2931,116 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="A14:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="rollNo" dataDxfId="23"/>
-    <tableColumn id="2" name="name" dataDxfId="22"/>
-    <tableColumn id="3" name="mobile" dataDxfId="21"/>
-    <tableColumn id="4" name="email" dataDxfId="20" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="deptNo" dataDxfId="19"/>
+    <tableColumn id="1" name="rollNo" dataDxfId="39"/>
+    <tableColumn id="2" name="name" dataDxfId="38"/>
+    <tableColumn id="3" name="mobile" dataDxfId="37"/>
+    <tableColumn id="4" name="email" dataDxfId="36" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="deptNo" dataDxfId="35"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="D116:E120" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="D116:E120"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Use Case" dataDxfId="3"/>
+    <tableColumn id="2" name="Grid Magic" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C26:E35" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C26:E35" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="C26:E35"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Selector Type" dataDxfId="8"/>
-    <tableColumn id="2" name="Example" dataDxfId="7"/>
-    <tableColumn id="3" name="Use Case" dataDxfId="6"/>
+    <tableColumn id="1" name="Selector Type" dataDxfId="32"/>
+    <tableColumn id="2" name="Example" dataDxfId="31"/>
+    <tableColumn id="3" name="Use Case" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C40:E45" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C40:E45" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
   <autoFilter ref="C40:E45"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Unit" dataDxfId="13"/>
-    <tableColumn id="2" name="Use Case" dataDxfId="12"/>
-    <tableColumn id="3" name="Example" dataDxfId="11"/>
+    <tableColumn id="1" name="Unit" dataDxfId="27"/>
+    <tableColumn id="2" name="Use Case" dataDxfId="26"/>
+    <tableColumn id="3" name="Example" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C59:E64" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C59:E64" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
   <autoFilter ref="C59:E64"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Feature" dataDxfId="18"/>
-    <tableColumn id="2" name="content-box (default)" dataDxfId="17"/>
-    <tableColumn id="3" name="border-box (modern layout favorite)" dataDxfId="16"/>
+    <tableColumn id="1" name="Feature" dataDxfId="22"/>
+    <tableColumn id="2" name="content-box (default)" dataDxfId="21"/>
+    <tableColumn id="3" name="border-box (modern layout favorite)" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C69:D74" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C69:D74" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="C69:D74"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Position Type" dataDxfId="3"/>
-    <tableColumn id="2" name="Description" dataDxfId="2"/>
+    <tableColumn id="1" name="Position Type" dataDxfId="17"/>
+    <tableColumn id="2" name="Description" dataDxfId="16"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D81:E86" totalsRowShown="0" headerRowDxfId="13">
+  <autoFilter ref="D81:E86"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Property" dataDxfId="15"/>
+    <tableColumn id="2" name="Description" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D90:E94" totalsRowShown="0" headerRowDxfId="10">
+  <autoFilter ref="D90:E94"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Property" dataDxfId="12"/>
+    <tableColumn id="2" name="Description" dataDxfId="11"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="D100:E105" totalsRowShown="0" headerRowDxfId="7">
+  <autoFilter ref="D100:E105"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Property" dataDxfId="9"/>
+    <tableColumn id="2" name="Purpose" dataDxfId="8"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="D109:E112" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="D109:E112"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Property" dataDxfId="6"/>
+    <tableColumn id="2" name="Purpose" dataDxfId="5"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3219,8 +4069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3234,15 +4084,18 @@
       <c r="B2" s="2" t="s">
         <v>161</v>
       </c>
+      <c r="F2" s="1" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="3" spans="2:10">
-      <c r="F3" s="1" t="s">
+      <c r="F3" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="J3" s="3" t="s">
         <v>164</v>
       </c>
     </row>
@@ -3256,7 +4109,7 @@
       <c r="H4" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="J4" s="16" t="s">
         <v>168</v>
       </c>
     </row>
@@ -3274,10 +4127,10 @@
       <c r="B7" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="F7" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="H7" s="1" t="s">
+      <c r="H7" s="16" t="s">
         <v>173</v>
       </c>
     </row>
@@ -3286,6 +4139,11 @@
         <v>174</v>
       </c>
     </row>
+    <row r="9" spans="2:10">
+      <c r="F9" s="1" t="s">
+        <v>311</v>
+      </c>
+    </row>
     <row r="11" spans="2:10">
       <c r="B11" s="2" t="s">
         <v>175</v>
@@ -3389,7 +4247,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="33" spans="2:3">
+    <row r="33" spans="2:6">
       <c r="B33" s="1" t="s">
         <v>186</v>
       </c>
@@ -3397,111 +4255,122 @@
         <v>198</v>
       </c>
     </row>
-    <row r="34" spans="2:3">
+    <row r="34" spans="2:6">
       <c r="B34" s="1" t="s">
         <v>188</v>
       </c>
       <c r="C34" s="1" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6">
+      <c r="B36" s="2" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="36" spans="2:3">
-      <c r="B36" s="2" t="s">
+    <row r="37" spans="2:6">
+      <c r="F37" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6">
+      <c r="B38" s="1" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="2:3">
-      <c r="B38" s="1" t="s">
+      <c r="C38" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="C38" s="1" t="s">
+    </row>
+    <row r="39" spans="2:6">
+      <c r="B39" s="1" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="39" spans="2:3">
-      <c r="B39" s="1" t="s">
+      <c r="C39" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C39" s="1" t="s">
+      <c r="F39" s="6" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6">
+      <c r="B40" s="1" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="40" spans="2:3">
-      <c r="B40" s="1" t="s">
+      <c r="C40" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="C40" s="1" t="s">
+    </row>
+    <row r="41" spans="2:6">
+      <c r="B41" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="41" spans="2:3">
-      <c r="B41" s="1" t="s">
+      <c r="C41" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="C41" s="1" t="s">
+    </row>
+    <row r="42" spans="2:6">
+      <c r="B42" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="42" spans="2:3">
-      <c r="B42" s="1" t="s">
+      <c r="C42" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="C42" s="1" t="s">
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="2" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="45" spans="2:3">
-      <c r="B45" s="2" t="s">
+    <row r="47" spans="2:6">
+      <c r="B47" s="1" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="47" spans="2:3">
-      <c r="B47" s="1" t="s">
+    <row r="48" spans="2:6">
+      <c r="B48" s="1" t="s">
         <v>212</v>
-      </c>
-    </row>
-    <row r="48" spans="2:3">
-      <c r="B48" s="1" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="49" spans="2:2">
       <c r="B49" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="50" spans="2:2">
       <c r="B50" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="51" spans="2:2">
       <c r="B51" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="52" spans="2:2">
       <c r="B52" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="53" spans="2:2">
       <c r="B53" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F39" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E74"/>
+  <dimension ref="A1:E120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="C115" sqref="C115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3516,12 +4385,12 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="57.6">
       <c r="B3" s="9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3529,7 +4398,7 @@
     </row>
     <row r="5" spans="1:2" ht="43.2">
       <c r="B5" s="9" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3537,7 +4406,7 @@
     </row>
     <row r="7" spans="1:2" ht="43.2">
       <c r="B7" s="9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -3545,7 +4414,7 @@
     </row>
     <row r="9" spans="1:2" ht="43.2">
       <c r="B9" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -3553,7 +4422,7 @@
     </row>
     <row r="11" spans="1:2" ht="43.2">
       <c r="B11" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -3561,7 +4430,7 @@
     </row>
     <row r="13" spans="1:2" ht="28.8">
       <c r="B13" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -3569,7 +4438,7 @@
     </row>
     <row r="15" spans="1:2" ht="28.8">
       <c r="B15" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -3577,7 +4446,10 @@
     </row>
     <row r="17" spans="1:5" ht="28.8">
       <c r="B17" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -3590,183 +4462,183 @@
     </row>
     <row r="26" spans="1:5" ht="15" customHeight="1">
       <c r="C26" s="13" t="s">
+        <v>219</v>
+      </c>
+      <c r="D26" s="13" t="s">
         <v>220</v>
       </c>
-      <c r="D26" s="13" t="s">
+      <c r="E26" s="13" t="s">
         <v>221</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>222</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="15" customHeight="1">
       <c r="C27" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D27" s="8" t="s">
         <v>223</v>
       </c>
-      <c r="D27" s="8" t="s">
+      <c r="E27" s="15" t="s">
         <v>224</v>
-      </c>
-      <c r="E27" s="15" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="15" customHeight="1">
       <c r="C28" s="15" t="s">
+        <v>225</v>
+      </c>
+      <c r="D28" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="D28" s="8" t="s">
+      <c r="E28" s="15" t="s">
         <v>227</v>
-      </c>
-      <c r="E28" s="15" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="15" customHeight="1">
       <c r="C29" s="15" t="s">
+        <v>228</v>
+      </c>
+      <c r="D29" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="D29" s="8" t="s">
+      <c r="E29" s="15" t="s">
         <v>230</v>
-      </c>
-      <c r="E29" s="15" t="s">
-        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="15" customHeight="1">
       <c r="C30" s="15" t="s">
+        <v>231</v>
+      </c>
+      <c r="D30" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="15" t="s">
         <v>233</v>
-      </c>
-      <c r="E30" s="15" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="15" customHeight="1">
       <c r="C31" s="15" t="s">
+        <v>234</v>
+      </c>
+      <c r="D31" s="8" t="s">
         <v>235</v>
       </c>
-      <c r="D31" s="8" t="s">
-        <v>236</v>
-      </c>
       <c r="E31" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
       <c r="C32" s="15" t="s">
+        <v>236</v>
+      </c>
+      <c r="D32" s="8" t="s">
         <v>237</v>
       </c>
-      <c r="D32" s="8" t="s">
-        <v>238</v>
-      </c>
       <c r="E32" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="15" customHeight="1">
       <c r="C33" s="15" t="s">
+        <v>238</v>
+      </c>
+      <c r="D33" s="8" t="s">
         <v>239</v>
       </c>
-      <c r="D33" s="8" t="s">
-        <v>240</v>
-      </c>
       <c r="E33" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="15" customHeight="1">
       <c r="C34" s="15" t="s">
+        <v>240</v>
+      </c>
+      <c r="D34" s="8" t="s">
         <v>241</v>
       </c>
-      <c r="D34" s="8" t="s">
+      <c r="E34" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="E34" s="15" t="s">
+    </row>
+    <row r="35" spans="2:5" ht="36.6" customHeight="1">
+      <c r="C35" s="15" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" ht="15" customHeight="1">
-      <c r="C35" s="15" t="s">
+      <c r="D35" s="8" t="s">
         <v>244</v>
       </c>
-      <c r="D35" s="8" t="s">
+      <c r="E35" s="15" t="s">
         <v>245</v>
-      </c>
-      <c r="E35" s="15" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="11" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="40" spans="2:5">
       <c r="C40" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="41" spans="2:5">
       <c r="C41" s="8" t="s">
+        <v>256</v>
+      </c>
+      <c r="D41" s="15" t="s">
         <v>257</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="E41" s="8" t="s">
         <v>258</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="42" spans="2:5">
       <c r="C42" s="8" t="s">
+        <v>259</v>
+      </c>
+      <c r="D42" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="E42" s="8" t="s">
         <v>261</v>
-      </c>
-      <c r="E42" s="8" t="s">
-        <v>262</v>
       </c>
     </row>
     <row r="43" spans="2:5" ht="27.6">
       <c r="C43" s="8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D43" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="E43" s="8" t="s">
         <v>264</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="44" spans="2:5" ht="27.6">
       <c r="C44" s="8" t="s">
+        <v>265</v>
+      </c>
+      <c r="D44" s="15" t="s">
         <v>266</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="E44" s="8" t="s">
         <v>267</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>268</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="27.6">
       <c r="C45" s="8" t="s">
+        <v>268</v>
+      </c>
+      <c r="D45" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="E45" s="8" t="s">
         <v>270</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -3774,98 +4646,98 @@
         <v>2</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="28.8">
       <c r="B51" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.8">
       <c r="B53" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="28.8">
       <c r="B55" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8">
       <c r="B57" s="11" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="C58" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="27.6">
       <c r="C59" s="13" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D59" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>288</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>289</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="27.6">
       <c r="C60" s="14" t="s">
+        <v>289</v>
+      </c>
+      <c r="D60" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="E60" s="15" t="s">
         <v>291</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="27.6">
       <c r="C61" s="14" t="s">
+        <v>278</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>279</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>280</v>
-      </c>
       <c r="E61" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="55.2">
       <c r="C62" s="14" t="s">
+        <v>280</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="E62" s="15" t="s">
         <v>282</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>283</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="41.4">
       <c r="C63" s="14" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D63" s="15" t="s">
+        <v>293</v>
+      </c>
+      <c r="E63" s="15" t="s">
         <v>294</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>295</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="41.4">
       <c r="C64" s="14" t="s">
+        <v>284</v>
+      </c>
+      <c r="D64" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="E64" s="15" t="s">
         <v>286</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -3873,65 +4745,359 @@
         <v>3</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="C69" s="13" t="s">
+        <v>299</v>
+      </c>
+      <c r="D69" s="13" t="s">
         <v>300</v>
-      </c>
-      <c r="D69" s="13" t="s">
-        <v>301</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="27.6">
       <c r="C70" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>302</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>303</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="27.6">
       <c r="C71" s="8" t="s">
+        <v>303</v>
+      </c>
+      <c r="D71" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="D71" s="15" t="s">
+    </row>
+    <row r="72" spans="1:4" ht="55.2">
+      <c r="C72" s="8" t="s">
         <v>305</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="41.4">
-      <c r="C72" s="8" t="s">
-        <v>306</v>
-      </c>
       <c r="D72" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="41.4">
       <c r="C73" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="55.2">
       <c r="C74" s="8" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>311</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="2">
+        <v>4</v>
+      </c>
+      <c r="B78" s="11" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="B80" s="17" t="s">
+        <v>318</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="81" spans="2:5">
+      <c r="B81" s="18"/>
+      <c r="D81" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="E81" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="82" spans="2:5">
+      <c r="B82" s="22" t="s">
+        <v>321</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="E82" s="20" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="83" spans="2:5">
+      <c r="B83" s="21"/>
+      <c r="D83" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="84" spans="2:5">
+      <c r="B84" s="22" t="s">
+        <v>322</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="E84" s="20" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="2:5">
+      <c r="B85" s="23"/>
+      <c r="D85" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="E85" s="20" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="86" spans="2:5" ht="28.8">
+      <c r="B86" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>332</v>
+      </c>
+      <c r="E86" s="20" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="87" spans="2:5">
+      <c r="B87" s="23"/>
+    </row>
+    <row r="88" spans="2:5" ht="28.2">
+      <c r="B88" s="23" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="89" spans="2:5">
+      <c r="D89" s="1" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="90" spans="2:5">
+      <c r="D90" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="91" spans="2:5">
+      <c r="D91" s="8" t="s">
+        <v>334</v>
+      </c>
+      <c r="E91" s="20" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="92" spans="2:5">
+      <c r="D92" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="E92" s="20" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="93" spans="2:5">
+      <c r="D93" s="8" t="s">
+        <v>338</v>
+      </c>
+      <c r="E93" s="20" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="94" spans="2:5">
+      <c r="D94" s="8" t="s">
+        <v>340</v>
+      </c>
+      <c r="E94" s="20" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" s="2">
+        <v>5</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="D99" s="1" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" ht="28.8">
+      <c r="B100" s="21" t="s">
+        <v>347</v>
+      </c>
+      <c r="D100" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="E100" s="19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" ht="26.4">
+      <c r="B101" s="21"/>
+      <c r="D101" s="8" t="s">
+        <v>350</v>
+      </c>
+      <c r="E101" s="20" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5">
+      <c r="B102" s="21" t="s">
+        <v>345</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>352</v>
+      </c>
+      <c r="E102" s="20" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5">
+      <c r="B103" s="21"/>
+      <c r="D103" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E103" s="20" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" ht="26.4">
+      <c r="B104" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="D104" s="8" t="s">
+        <v>356</v>
+      </c>
+      <c r="E104" s="20" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" ht="42">
+      <c r="B105" s="21"/>
+      <c r="D105" s="8" t="s">
+        <v>358</v>
+      </c>
+      <c r="E105" s="20" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" ht="28.8">
+      <c r="B106" s="21" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5">
+      <c r="D108" s="1" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5">
+      <c r="D109" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="E109" s="19" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" ht="27.6">
+      <c r="D110" s="8" t="s">
+        <v>362</v>
+      </c>
+      <c r="E110" s="20" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5">
+      <c r="D111" s="8" t="s">
+        <v>364</v>
+      </c>
+      <c r="E111" s="20" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" ht="27.6">
+      <c r="D112" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="E112" s="20" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="115" spans="4:5">
+      <c r="D115" s="1" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="116" spans="4:5">
+      <c r="D116" s="19" t="s">
+        <v>221</v>
+      </c>
+      <c r="E116" s="19" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="117" spans="4:5">
+      <c r="D117" s="20" t="s">
+        <v>370</v>
+      </c>
+      <c r="E117" s="20" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="118" spans="4:5">
+      <c r="D118" s="20" t="s">
+        <v>372</v>
+      </c>
+      <c r="E118" s="20" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="119" spans="4:5">
+      <c r="D119" s="20" t="s">
+        <v>374</v>
+      </c>
+      <c r="E119" s="20" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="120" spans="4:5">
+      <c r="D120" s="20" t="s">
+        <v>376</v>
+      </c>
+      <c r="E120" s="20" t="s">
+        <v>377</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="4">
+  <tableParts count="9">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
+    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId9"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat(css): added animation, transition, and media query demo files chore(css): updated box model, z-index, and selector/unit examples docs: modified class_notes.xlsx to reflect new CSS topics
</commit_message>
<xml_diff>
--- a/1_Materials/classNotes/class_notes.xlsx
+++ b/1_Materials/classNotes/class_notes.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="378">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="512" uniqueCount="473">
   <si>
     <t>DATABASE</t>
   </si>
@@ -1062,9 +1062,6 @@
     <t>rem</t>
   </si>
   <si>
-    <t>Relative to root font size</t>
-  </si>
-  <si>
     <t>font-size: 1.5rem</t>
   </si>
   <si>
@@ -2145,6 +2142,589 @@
   </si>
   <si>
     <t>Skip flex nesting madness</t>
+  </si>
+  <si>
+    <t>inline
+internal
+external</t>
+  </si>
+  <si>
+    <t>Relative to root font size - &lt;html&gt;</t>
+  </si>
+  <si>
+    <t>TRANSITION</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">animates the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>change</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> from one property value to another over time.</t>
+    </r>
+  </si>
+  <si>
+    <t>selector {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  transition: property duration timing-function delay;</t>
+  </si>
+  <si>
+    <t>}</t>
+  </si>
+  <si>
+    <t>Syntax</t>
+  </si>
+  <si>
+    <t>button {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  transition: background-color 0.3s ease;</t>
+  </si>
+  <si>
+    <t>Effect</t>
+  </si>
+  <si>
+    <t>background-color</t>
+  </si>
+  <si>
+    <t>Hover glow/buttons</t>
+  </si>
+  <si>
+    <t>color</t>
+  </si>
+  <si>
+    <t>Text fade</t>
+  </si>
+  <si>
+    <t>transform</t>
+  </si>
+  <si>
+    <t>Scale/rotate/shift</t>
+  </si>
+  <si>
+    <t>opacity</t>
+  </si>
+  <si>
+    <t>Fades in/out</t>
+  </si>
+  <si>
+    <t>box-shadow</t>
+  </si>
+  <si>
+    <t>Soft shadows on hover</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>linear</t>
+  </si>
+  <si>
+    <t>Same speed throughout</t>
+  </si>
+  <si>
+    <t>ease</t>
+  </si>
+  <si>
+    <t>Start slow, speed up, slow end (default)</t>
+  </si>
+  <si>
+    <t>ease-in</t>
+  </si>
+  <si>
+    <t>Starts slow</t>
+  </si>
+  <si>
+    <t>ease-out</t>
+  </si>
+  <si>
+    <t>Ends slow</t>
+  </si>
+  <si>
+    <t>ease-in-out</t>
+  </si>
+  <si>
+    <t>Slow start and end</t>
+  </si>
+  <si>
+    <t>cubic-bezier(...)</t>
+  </si>
+  <si>
+    <t>Custom motion curve (advanced)</t>
+  </si>
+  <si>
+    <t>ANIMATION</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">let you </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>define motion over time</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> using:</t>
+    </r>
+  </si>
+  <si>
+    <t>@keyframes slideIn {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  from {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    transform: translateX(-100%);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  to {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    transform: translateX(0);</t>
+  </si>
+  <si>
+    <t>1. @keyframes — Defines the stages of animation</t>
+  </si>
+  <si>
+    <t>2. animation — Applies the animation to elements</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  animation: name duration timing-function delay iteration-count direction;</t>
+  </si>
+  <si>
+    <t>What it does</t>
+  </si>
+  <si>
+    <t>animation-name</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Refers to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>@keyframes</t>
+    </r>
+  </si>
+  <si>
+    <t>animation-duration</t>
+  </si>
+  <si>
+    <t>Time to complete one cycle</t>
+  </si>
+  <si>
+    <t>animation-delay</t>
+  </si>
+  <si>
+    <t>Wait before starting</t>
+  </si>
+  <si>
+    <t>animation-iteration-count</t>
+  </si>
+  <si>
+    <r>
+      <t>1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>infinite</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, or a number</t>
+    </r>
+  </si>
+  <si>
+    <t>animation-direction</t>
+  </si>
+  <si>
+    <r>
+      <t>normal</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>alternate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, etc.</t>
+    </r>
+  </si>
+  <si>
+    <t>animation-fill-mode</t>
+  </si>
+  <si>
+    <r>
+      <t>forwards</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>backwards</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial Unicode MS"/>
+      </rPr>
+      <t>both</t>
+    </r>
+  </si>
+  <si>
+    <t>MEDIA QUERIES</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">let you apply </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>different CSS rules</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> based on:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">They help build </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>mobile-first</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>responsive layouts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Screen width</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Device </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>type</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Display </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>resolution</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Orientation (landscape/portrait)</t>
+  </si>
+  <si>
+    <t>@media (condition) {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  /* styles for when condition is true */</t>
+  </si>
+  <si>
+    <t>Condition</t>
+  </si>
+  <si>
+    <t>Meaning</t>
+  </si>
+  <si>
+    <t>max-width: 600px</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Devices </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>up to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 600px wide (mobile)</t>
+    </r>
+  </si>
+  <si>
+    <t>min-width: 768px</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Devices </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>from</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 768px and above</t>
+    </r>
+  </si>
+  <si>
+    <t>orientation: landscape</t>
+  </si>
+  <si>
+    <t>Wide screen orientation</t>
+  </si>
+  <si>
+    <t>Alias</t>
+  </si>
+  <si>
+    <t>Range (px)</t>
+  </si>
+  <si>
+    <t>Usage Example</t>
+  </si>
+  <si>
+    <t>xs</t>
+  </si>
+  <si>
+    <t>&lt;576px</t>
+  </si>
+  <si>
+    <t>Mobile phones (portrait)</t>
+  </si>
+  <si>
+    <t>sm</t>
+  </si>
+  <si>
+    <t>≥576px</t>
+  </si>
+  <si>
+    <t>Phones (landscape)</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t>≥768px</t>
+  </si>
+  <si>
+    <t>Tablets</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>≥992px</t>
+  </si>
+  <si>
+    <t>Small desktops</t>
+  </si>
+  <si>
+    <t>xl</t>
+  </si>
+  <si>
+    <t>≥1200px</t>
+  </si>
+  <si>
+    <t>Large desktops</t>
+  </si>
+  <si>
+    <t>xxl</t>
+  </si>
+  <si>
+    <t>≥1400px</t>
+  </si>
+  <si>
+    <t>Extra large screens / 4K TVs</t>
   </si>
 </sst>
 </file>
@@ -2230,13 +2810,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -2247,8 +2820,16 @@
       <color theme="1"/>
       <name val="Arial Unicode MS"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2271,8 +2852,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -2280,14 +2866,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2342,14 +2944,30 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="1" xfId="4" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Calculation" xfId="4" builtinId="22"/>
     <cellStyle name="Good" xfId="3" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="42">
+  <dxfs count="59">
     <dxf>
       <font>
         <b/>
@@ -2367,6 +2985,234 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Arial Unicode MS"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -2532,6 +3378,24 @@
         <scheme val="none"/>
       </font>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -2931,116 +3795,172 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A14:E16" totalsRowShown="0" headerRowDxfId="58" dataDxfId="57">
   <autoFilter ref="A14:E16"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="rollNo" dataDxfId="39"/>
-    <tableColumn id="2" name="name" dataDxfId="38"/>
-    <tableColumn id="3" name="mobile" dataDxfId="37"/>
-    <tableColumn id="4" name="email" dataDxfId="36" dataCellStyle="Hyperlink"/>
-    <tableColumn id="5" name="deptNo" dataDxfId="35"/>
+    <tableColumn id="1" name="rollNo" dataDxfId="56"/>
+    <tableColumn id="2" name="name" dataDxfId="55"/>
+    <tableColumn id="3" name="mobile" dataDxfId="54"/>
+    <tableColumn id="4" name="email" dataDxfId="53" dataCellStyle="Hyperlink"/>
+    <tableColumn id="5" name="deptNo" dataDxfId="52"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="D116:E120" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table10" displayName="Table10" ref="D116:E120" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
   <autoFilter ref="D116:E120"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Use Case" dataDxfId="3"/>
-    <tableColumn id="2" name="Grid Magic" dataDxfId="2"/>
+    <tableColumn id="1" name="Use Case" dataDxfId="18"/>
+    <tableColumn id="2" name="Grid Magic" dataDxfId="17"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table11" displayName="Table11" ref="D137:E142" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="D137:E142"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Property" dataDxfId="16"/>
+    <tableColumn id="2" name="Effect" dataDxfId="15"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table12" displayName="Table12" ref="D145:E151" totalsRowShown="0" headerRowDxfId="11">
+  <autoFilter ref="D145:E151"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Function" dataDxfId="13"/>
+    <tableColumn id="2" name="Description" dataDxfId="12"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table13.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table13" displayName="Table13" ref="D175:E181" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
+  <autoFilter ref="D175:E181"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Property" dataDxfId="10"/>
+    <tableColumn id="2" name="What it does" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table14.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="14" name="Table14" displayName="Table14" ref="D203:E206" totalsRowShown="0" headerRowDxfId="4">
+  <autoFilter ref="D203:E206"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Condition" dataDxfId="6"/>
+    <tableColumn id="2" name="Meaning" dataDxfId="5"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table15.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="15" name="Table15" displayName="Table15" ref="C209:E215" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="C209:E215"/>
+  <tableColumns count="3">
+    <tableColumn id="1" name="Alias" dataDxfId="3"/>
+    <tableColumn id="2" name="Range (px)" dataDxfId="2"/>
+    <tableColumn id="3" name="Usage Example" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C26:E35" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="C26:E35" totalsRowShown="0" headerRowDxfId="51" dataDxfId="50">
   <autoFilter ref="C26:E35"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Selector Type" dataDxfId="32"/>
-    <tableColumn id="2" name="Example" dataDxfId="31"/>
-    <tableColumn id="3" name="Use Case" dataDxfId="30"/>
+    <tableColumn id="1" name="Selector Type" dataDxfId="49"/>
+    <tableColumn id="2" name="Example" dataDxfId="48"/>
+    <tableColumn id="3" name="Use Case" dataDxfId="47"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C40:E45" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="C40:E45" totalsRowShown="0" headerRowDxfId="46" dataDxfId="45">
   <autoFilter ref="C40:E45"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Unit" dataDxfId="27"/>
-    <tableColumn id="2" name="Use Case" dataDxfId="26"/>
-    <tableColumn id="3" name="Example" dataDxfId="25"/>
+    <tableColumn id="1" name="Unit" dataDxfId="44"/>
+    <tableColumn id="2" name="Use Case" dataDxfId="43"/>
+    <tableColumn id="3" name="Example" dataDxfId="42"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C59:E64" totalsRowShown="0" headerRowDxfId="24" dataDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="C59:E64" totalsRowShown="0" headerRowDxfId="41" dataDxfId="40">
   <autoFilter ref="C59:E64"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Feature" dataDxfId="22"/>
-    <tableColumn id="2" name="content-box (default)" dataDxfId="21"/>
-    <tableColumn id="3" name="border-box (modern layout favorite)" dataDxfId="20"/>
+    <tableColumn id="1" name="Feature" dataDxfId="39"/>
+    <tableColumn id="2" name="content-box (default)" dataDxfId="38"/>
+    <tableColumn id="3" name="border-box (modern layout favorite)" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C69:D74" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table5" displayName="Table5" ref="C69:D74" totalsRowShown="0" headerRowDxfId="36" dataDxfId="35">
   <autoFilter ref="C69:D74"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Position Type" dataDxfId="17"/>
-    <tableColumn id="2" name="Description" dataDxfId="16"/>
+    <tableColumn id="1" name="Position Type" dataDxfId="34"/>
+    <tableColumn id="2" name="Description" dataDxfId="33"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D81:E86" totalsRowShown="0" headerRowDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="D81:E86" totalsRowShown="0" headerRowDxfId="32">
   <autoFilter ref="D81:E86"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Property" dataDxfId="15"/>
-    <tableColumn id="2" name="Description" dataDxfId="14"/>
+    <tableColumn id="1" name="Property" dataDxfId="31"/>
+    <tableColumn id="2" name="Description" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D90:E94" totalsRowShown="0" headerRowDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table7" displayName="Table7" ref="D90:E94" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="D90:E94"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Property" dataDxfId="12"/>
-    <tableColumn id="2" name="Description" dataDxfId="11"/>
+    <tableColumn id="1" name="Property" dataDxfId="28"/>
+    <tableColumn id="2" name="Description" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="D100:E105" totalsRowShown="0" headerRowDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table8" displayName="Table8" ref="D100:E105" totalsRowShown="0" headerRowDxfId="26">
   <autoFilter ref="D100:E105"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Property" dataDxfId="9"/>
-    <tableColumn id="2" name="Purpose" dataDxfId="8"/>
+    <tableColumn id="1" name="Property" dataDxfId="25"/>
+    <tableColumn id="2" name="Purpose" dataDxfId="24"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="D109:E112" totalsRowShown="0" headerRowDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table9" displayName="Table9" ref="D109:E112" totalsRowShown="0" headerRowDxfId="23">
   <autoFilter ref="D109:E112"/>
   <tableColumns count="2">
-    <tableColumn id="1" name="Property" dataDxfId="6"/>
-    <tableColumn id="2" name="Purpose" dataDxfId="5"/>
+    <tableColumn id="1" name="Property" dataDxfId="22"/>
+    <tableColumn id="2" name="Purpose" dataDxfId="21"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium5" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4069,8 +4989,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J53"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -4085,7 +5005,7 @@
         <v>161</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="3" spans="2:10">
@@ -4141,7 +5061,7 @@
     </row>
     <row r="9" spans="2:10">
       <c r="F9" s="1" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="11" spans="2:10">
@@ -4260,7 +5180,7 @@
         <v>188</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="36" spans="2:6">
@@ -4270,7 +5190,7 @@
     </row>
     <row r="37" spans="2:6">
       <c r="F37" s="1" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="38" spans="2:6">
@@ -4289,7 +5209,7 @@
         <v>203</v>
       </c>
       <c r="F39" s="6" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="40" spans="2:6">
@@ -4367,81 +5287,82 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E120"/>
+  <dimension ref="A1:E215"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A108" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C115" sqref="C115"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
     <col min="2" max="2" width="28.21875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="16.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.77734375" style="1" customWidth="1"/>
     <col min="4" max="4" width="16.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="39.109375" style="1" customWidth="1"/>
     <col min="6" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="57.6">
+    <row r="3" spans="1:4" ht="57.6">
       <c r="B3" s="9" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="D3" s="5" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" ht="43.2">
+    <row r="5" spans="1:4" ht="43.2">
       <c r="B5" s="9" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:4">
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" ht="43.2">
+    <row r="7" spans="1:4" ht="43.2">
       <c r="B7" s="9" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:4">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" ht="43.2">
+    <row r="9" spans="1:4" ht="43.2">
       <c r="B9" s="9" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="10" spans="1:2">
+    <row r="10" spans="1:4">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" ht="43.2">
+    <row r="11" spans="1:4" ht="43.2">
       <c r="B11" s="9" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:4">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" ht="28.8">
+    <row r="13" spans="1:4" ht="28.8">
       <c r="B13" s="9" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:4">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" ht="28.8">
+    <row r="15" spans="1:4" ht="28.8">
       <c r="B15" s="9" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:4">
       <c r="B16" s="10"/>
     </row>
     <row r="17" spans="1:5" ht="28.8">
@@ -4449,7 +5370,7 @@
         <v>253</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -4523,7 +5444,7 @@
         <v>235</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="15" customHeight="1">
@@ -4534,7 +5455,7 @@
         <v>237</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="33" spans="2:5" ht="15" customHeight="1">
@@ -4545,7 +5466,7 @@
         <v>239</v>
       </c>
       <c r="E33" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="34" spans="2:5" ht="15" customHeight="1">
@@ -4624,21 +5545,21 @@
         <v>265</v>
       </c>
       <c r="D44" s="15" t="s">
+        <v>378</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>266</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="45" spans="2:5" ht="27.6">
       <c r="C45" s="8" t="s">
+        <v>267</v>
+      </c>
+      <c r="D45" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="E45" s="8" t="s">
         <v>269</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>270</v>
       </c>
     </row>
     <row r="49" spans="1:5">
@@ -4646,98 +5567,98 @@
         <v>2</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="51" spans="1:5" ht="28.8">
       <c r="B51" s="11" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="53" spans="1:5" ht="28.8">
       <c r="B53" s="11" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="55" spans="1:5" ht="28.8">
       <c r="B55" s="11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="57" spans="1:5" ht="28.8">
       <c r="B57" s="11" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="C58" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="59" spans="1:5" ht="27.6">
       <c r="C59" s="13" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D59" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="E59" s="12" t="s">
         <v>287</v>
-      </c>
-      <c r="E59" s="12" t="s">
-        <v>288</v>
       </c>
     </row>
     <row r="60" spans="1:5" ht="27.6">
       <c r="C60" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="D60" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="E60" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="E60" s="15" t="s">
-        <v>291</v>
       </c>
     </row>
     <row r="61" spans="1:5" ht="27.6">
       <c r="C61" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>278</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>279</v>
-      </c>
       <c r="E61" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="62" spans="1:5" ht="55.2">
       <c r="C62" s="14" t="s">
+        <v>279</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="D62" s="15" t="s">
+      <c r="E62" s="15" t="s">
         <v>281</v>
-      </c>
-      <c r="E62" s="15" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="63" spans="1:5" ht="41.4">
       <c r="C63" s="14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D63" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="E63" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="E63" s="15" t="s">
-        <v>294</v>
       </c>
     </row>
     <row r="64" spans="1:5" ht="41.4">
       <c r="C64" s="14" t="s">
+        <v>283</v>
+      </c>
+      <c r="D64" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="D64" s="15" t="s">
+      <c r="E64" s="15" t="s">
         <v>285</v>
-      </c>
-      <c r="E64" s="15" t="s">
-        <v>286</v>
       </c>
     </row>
     <row r="68" spans="1:4">
@@ -4745,55 +5666,55 @@
         <v>3</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="69" spans="1:4">
       <c r="C69" s="13" t="s">
+        <v>298</v>
+      </c>
+      <c r="D69" s="13" t="s">
         <v>299</v>
-      </c>
-      <c r="D69" s="13" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="70" spans="1:4" ht="27.6">
       <c r="C70" s="8" t="s">
+        <v>300</v>
+      </c>
+      <c r="D70" s="15" t="s">
         <v>301</v>
-      </c>
-      <c r="D70" s="15" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="27.6">
       <c r="C71" s="8" t="s">
+        <v>302</v>
+      </c>
+      <c r="D71" s="15" t="s">
         <v>303</v>
-      </c>
-      <c r="D71" s="15" t="s">
-        <v>304</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="55.2">
       <c r="C72" s="8" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="73" spans="1:4" ht="41.4">
       <c r="C73" s="8" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D73" s="15" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="74" spans="1:4" ht="55.2">
       <c r="C74" s="8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D74" s="15" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="78" spans="1:4">
@@ -4801,75 +5722,75 @@
         <v>4</v>
       </c>
       <c r="B78" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="B80" s="17" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="81" spans="2:5">
       <c r="B81" s="18"/>
       <c r="D81" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E81" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="82" spans="2:5">
       <c r="B82" s="22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D82" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="E82" s="20" t="s">
         <v>324</v>
-      </c>
-      <c r="E82" s="20" t="s">
-        <v>325</v>
       </c>
     </row>
     <row r="83" spans="2:5">
       <c r="B83" s="21"/>
       <c r="D83" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="E83" s="8" t="s">
         <v>326</v>
-      </c>
-      <c r="E83" s="8" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" s="22" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D84" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="E84" s="20" t="s">
         <v>328</v>
-      </c>
-      <c r="E84" s="20" t="s">
-        <v>329</v>
       </c>
     </row>
     <row r="85" spans="2:5">
       <c r="B85" s="23"/>
       <c r="D85" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="E85" s="20" t="s">
         <v>330</v>
-      </c>
-      <c r="E85" s="20" t="s">
-        <v>331</v>
       </c>
     </row>
     <row r="86" spans="2:5" ht="28.8">
       <c r="B86" s="9" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D86" s="8" t="s">
+        <v>331</v>
+      </c>
+      <c r="E86" s="20" t="s">
         <v>332</v>
-      </c>
-      <c r="E86" s="20" t="s">
-        <v>333</v>
       </c>
     </row>
     <row r="87" spans="2:5">
@@ -4877,52 +5798,52 @@
     </row>
     <row r="88" spans="2:5" ht="28.2">
       <c r="B88" s="23" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="89" spans="2:5">
       <c r="D89" s="1" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="90" spans="2:5">
       <c r="D90" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E90" s="19" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="91" spans="2:5">
       <c r="D91" s="8" t="s">
+        <v>333</v>
+      </c>
+      <c r="E91" s="20" t="s">
         <v>334</v>
-      </c>
-      <c r="E91" s="20" t="s">
-        <v>335</v>
       </c>
     </row>
     <row r="92" spans="2:5">
       <c r="D92" s="8" t="s">
+        <v>335</v>
+      </c>
+      <c r="E92" s="20" t="s">
         <v>336</v>
-      </c>
-      <c r="E92" s="20" t="s">
-        <v>337</v>
       </c>
     </row>
     <row r="93" spans="2:5">
       <c r="D93" s="8" t="s">
+        <v>337</v>
+      </c>
+      <c r="E93" s="20" t="s">
         <v>338</v>
-      </c>
-      <c r="E93" s="20" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="94" spans="2:5">
       <c r="D94" s="8" t="s">
+        <v>339</v>
+      </c>
+      <c r="E94" s="20" t="s">
         <v>340</v>
-      </c>
-      <c r="E94" s="20" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -4930,165 +5851,645 @@
         <v>5</v>
       </c>
       <c r="B98" s="11" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="D99" s="1" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="100" spans="1:5" ht="28.8">
       <c r="B100" s="21" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="D100" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E100" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="101" spans="1:5" ht="26.4">
       <c r="B101" s="21"/>
       <c r="D101" s="8" t="s">
+        <v>349</v>
+      </c>
+      <c r="E101" s="20" t="s">
         <v>350</v>
-      </c>
-      <c r="E101" s="20" t="s">
-        <v>351</v>
       </c>
     </row>
     <row r="102" spans="1:5">
       <c r="B102" s="21" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D102" s="8" t="s">
+        <v>351</v>
+      </c>
+      <c r="E102" s="20" t="s">
         <v>352</v>
-      </c>
-      <c r="E102" s="20" t="s">
-        <v>353</v>
       </c>
     </row>
     <row r="103" spans="1:5">
       <c r="B103" s="21"/>
       <c r="D103" s="8" t="s">
+        <v>353</v>
+      </c>
+      <c r="E103" s="20" t="s">
         <v>354</v>
-      </c>
-      <c r="E103" s="20" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="104" spans="1:5" ht="26.4">
       <c r="B104" s="21" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="D104" s="8" t="s">
+        <v>355</v>
+      </c>
+      <c r="E104" s="20" t="s">
         <v>356</v>
-      </c>
-      <c r="E104" s="20" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="105" spans="1:5" ht="42">
       <c r="B105" s="21"/>
       <c r="D105" s="8" t="s">
+        <v>357</v>
+      </c>
+      <c r="E105" s="20" t="s">
         <v>358</v>
-      </c>
-      <c r="E105" s="20" t="s">
-        <v>359</v>
       </c>
     </row>
     <row r="106" spans="1:5" ht="28.8">
       <c r="B106" s="21" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="108" spans="1:5">
       <c r="D108" s="1" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="109" spans="1:5">
       <c r="D109" s="19" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E109" s="19" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="110" spans="1:5" ht="27.6">
       <c r="D110" s="8" t="s">
+        <v>361</v>
+      </c>
+      <c r="E110" s="20" t="s">
         <v>362</v>
-      </c>
-      <c r="E110" s="20" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="111" spans="1:5">
       <c r="D111" s="8" t="s">
+        <v>363</v>
+      </c>
+      <c r="E111" s="20" t="s">
         <v>364</v>
-      </c>
-      <c r="E111" s="20" t="s">
-        <v>365</v>
       </c>
     </row>
     <row r="112" spans="1:5" ht="27.6">
       <c r="D112" s="8" t="s">
+        <v>365</v>
+      </c>
+      <c r="E112" s="20" t="s">
         <v>366</v>
       </c>
-      <c r="E112" s="20" t="s">
+    </row>
+    <row r="115" spans="1:5">
+      <c r="D115" s="1" t="s">
         <v>367</v>
       </c>
     </row>
-    <row r="115" spans="4:5">
-      <c r="D115" s="1" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="116" spans="4:5">
+    <row r="116" spans="1:5">
       <c r="D116" s="19" t="s">
         <v>221</v>
       </c>
       <c r="E116" s="19" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="117" spans="1:5">
+      <c r="D117" s="20" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="117" spans="4:5">
-      <c r="D117" s="20" t="s">
+      <c r="E117" s="20" t="s">
         <v>370</v>
       </c>
-      <c r="E117" s="20" t="s">
+    </row>
+    <row r="118" spans="1:5">
+      <c r="D118" s="20" t="s">
         <v>371</v>
       </c>
-    </row>
-    <row r="118" spans="4:5">
-      <c r="D118" s="20" t="s">
+      <c r="E118" s="20" t="s">
         <v>372</v>
       </c>
-      <c r="E118" s="20" t="s">
+    </row>
+    <row r="119" spans="1:5">
+      <c r="D119" s="20" t="s">
         <v>373</v>
       </c>
-    </row>
-    <row r="119" spans="4:5">
-      <c r="D119" s="20" t="s">
+      <c r="E119" s="20" t="s">
         <v>374</v>
       </c>
-      <c r="E119" s="20" t="s">
+    </row>
+    <row r="120" spans="1:5">
+      <c r="D120" s="20" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="120" spans="4:5">
-      <c r="D120" s="20" t="s">
+      <c r="E120" s="20" t="s">
         <v>376</v>
       </c>
-      <c r="E120" s="20" t="s">
-        <v>377</v>
+    </row>
+    <row r="123" spans="1:5">
+      <c r="A123" s="2">
+        <v>6</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="126" spans="1:5" ht="43.2">
+      <c r="B126" s="24" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="B128" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="129" spans="2:5">
+      <c r="B129" s="5" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="130" spans="2:5">
+      <c r="B130" s="5" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="131" spans="2:5">
+      <c r="B131" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="133" spans="2:5">
+      <c r="B133" s="25" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="134" spans="2:5">
+      <c r="B134" s="5" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="135" spans="2:5">
+      <c r="B135" s="5" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="136" spans="2:5">
+      <c r="B136" s="5" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="137" spans="2:5">
+      <c r="D137" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="E137" s="19" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="138" spans="2:5">
+      <c r="D138" s="8" t="s">
+        <v>388</v>
+      </c>
+      <c r="E138" s="20" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="139" spans="2:5">
+      <c r="D139" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="E139" s="20" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="140" spans="2:5">
+      <c r="D140" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="E140" s="20" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="141" spans="2:5">
+      <c r="D141" s="8" t="s">
+        <v>394</v>
+      </c>
+      <c r="E141" s="20" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="142" spans="2:5">
+      <c r="D142" s="8" t="s">
+        <v>396</v>
+      </c>
+      <c r="E142" s="20" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="145" spans="1:5">
+      <c r="D145" s="19" t="s">
+        <v>398</v>
+      </c>
+      <c r="E145" s="19" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="146" spans="1:5">
+      <c r="D146" s="8" t="s">
+        <v>399</v>
+      </c>
+      <c r="E146" s="20" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="147" spans="1:5">
+      <c r="D147" s="8" t="s">
+        <v>401</v>
+      </c>
+      <c r="E147" s="20" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="148" spans="1:5">
+      <c r="D148" s="8" t="s">
+        <v>403</v>
+      </c>
+      <c r="E148" s="20" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="149" spans="1:5">
+      <c r="D149" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="E149" s="20" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="150" spans="1:5">
+      <c r="D150" s="8" t="s">
+        <v>407</v>
+      </c>
+      <c r="E150" s="20" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="151" spans="1:5">
+      <c r="D151" s="8" t="s">
+        <v>409</v>
+      </c>
+      <c r="E151" s="20" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="153" spans="1:5">
+      <c r="A153" s="2">
+        <v>7</v>
+      </c>
+      <c r="B153" s="11" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="156" spans="1:5" ht="28.8">
+      <c r="B156" s="5" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="157" spans="1:5">
+      <c r="B157" s="10"/>
+    </row>
+    <row r="158" spans="1:5" ht="28.8">
+      <c r="B158" s="28" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="159" spans="1:5">
+      <c r="B159" s="10"/>
+    </row>
+    <row r="160" spans="1:5">
+      <c r="B160" s="27" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="161" spans="2:5">
+      <c r="B161" s="27" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="162" spans="2:5">
+      <c r="B162" s="27" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="163" spans="2:5">
+      <c r="B163" s="27" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="164" spans="2:5">
+      <c r="B164" s="27" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5">
+      <c r="B165" s="27" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="166" spans="2:5">
+      <c r="B166" s="27" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="167" spans="2:5">
+      <c r="B167" s="27" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="168" spans="2:5">
+      <c r="B168" s="27"/>
+    </row>
+    <row r="169" spans="2:5" ht="28.8">
+      <c r="B169" s="28" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="172" spans="2:5">
+      <c r="B172" s="1" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="173" spans="2:5">
+      <c r="B173" s="1" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="174" spans="2:5">
+      <c r="B174" s="1" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="175" spans="2:5">
+      <c r="D175" s="19" t="s">
+        <v>322</v>
+      </c>
+      <c r="E175" s="19" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="176" spans="2:5">
+      <c r="D176" s="8" t="s">
+        <v>423</v>
+      </c>
+      <c r="E176" s="20" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="177" spans="1:5">
+      <c r="D177" s="8" t="s">
+        <v>425</v>
+      </c>
+      <c r="E177" s="20" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="178" spans="1:5">
+      <c r="D178" s="8" t="s">
+        <v>427</v>
+      </c>
+      <c r="E178" s="20" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="179" spans="1:5" ht="26.4">
+      <c r="D179" s="8" t="s">
+        <v>429</v>
+      </c>
+      <c r="E179" s="8" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="180" spans="1:5">
+      <c r="D180" s="8" t="s">
+        <v>431</v>
+      </c>
+      <c r="E180" s="8" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="181" spans="1:5">
+      <c r="D181" s="8" t="s">
+        <v>433</v>
+      </c>
+      <c r="E181" s="8" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="186" spans="1:5">
+      <c r="A186" s="2">
+        <v>8</v>
+      </c>
+      <c r="B186" s="11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="188" spans="1:5">
+      <c r="B188" s="1" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="189" spans="1:5">
+      <c r="B189" s="26"/>
+    </row>
+    <row r="190" spans="1:5">
+      <c r="B190" s="26" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="191" spans="1:5">
+      <c r="B191" s="26"/>
+    </row>
+    <row r="192" spans="1:5">
+      <c r="B192" s="26" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="193" spans="2:5">
+      <c r="B193" s="26"/>
+    </row>
+    <row r="194" spans="2:5">
+      <c r="B194" s="26" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="195" spans="2:5">
+      <c r="B195" s="26"/>
+    </row>
+    <row r="196" spans="2:5">
+      <c r="B196" s="26" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="197" spans="2:5">
+      <c r="B197" s="1"/>
+    </row>
+    <row r="198" spans="2:5">
+      <c r="B198" s="1" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="200" spans="2:5">
+      <c r="B200" s="25" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="201" spans="2:5">
+      <c r="B201" s="5" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="202" spans="2:5" ht="28.8">
+      <c r="B202" s="5" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="203" spans="2:5">
+      <c r="B203" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="D203" s="19" t="s">
+        <v>444</v>
+      </c>
+      <c r="E203" s="19" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="204" spans="2:5">
+      <c r="D204" s="8" t="s">
+        <v>446</v>
+      </c>
+      <c r="E204" s="20" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="205" spans="2:5">
+      <c r="D205" s="8" t="s">
+        <v>448</v>
+      </c>
+      <c r="E205" s="20" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="206" spans="2:5" ht="26.4">
+      <c r="D206" s="8" t="s">
+        <v>450</v>
+      </c>
+      <c r="E206" s="20" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="209" spans="3:5">
+      <c r="C209" s="19" t="s">
+        <v>452</v>
+      </c>
+      <c r="D209" s="19" t="s">
+        <v>453</v>
+      </c>
+      <c r="E209" s="19" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="210" spans="3:5">
+      <c r="C210" s="8" t="s">
+        <v>455</v>
+      </c>
+      <c r="D210" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="E210" s="20" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="211" spans="3:5">
+      <c r="C211" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="D211" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="E211" s="20" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="212" spans="3:5">
+      <c r="C212" s="8" t="s">
+        <v>461</v>
+      </c>
+      <c r="D212" s="8" t="s">
+        <v>462</v>
+      </c>
+      <c r="E212" s="20" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="213" spans="3:5">
+      <c r="C213" s="8" t="s">
+        <v>464</v>
+      </c>
+      <c r="D213" s="8" t="s">
+        <v>465</v>
+      </c>
+      <c r="E213" s="20" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="214" spans="3:5">
+      <c r="C214" s="8" t="s">
+        <v>467</v>
+      </c>
+      <c r="D214" s="8" t="s">
+        <v>468</v>
+      </c>
+      <c r="E214" s="20" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="215" spans="3:5">
+      <c r="C215" s="8" t="s">
+        <v>470</v>
+      </c>
+      <c r="D215" s="8" t="s">
+        <v>471</v>
+      </c>
+      <c r="E215" s="20" t="s">
+        <v>472</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="9">
+  <tableParts count="14">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
@@ -5098,6 +6499,11 @@
     <tablePart r:id="rId8"/>
     <tablePart r:id="rId9"/>
     <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId12"/>
+    <tablePart r:id="rId13"/>
+    <tablePart r:id="rId14"/>
+    <tablePart r:id="rId15"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>